<commit_message>
filled in the observable list
</commit_message>
<xml_diff>
--- a/java/RoperALZIntake/RoperSpreadSheet2.xlsx
+++ b/java/RoperALZIntake/RoperSpreadSheet2.xlsx
@@ -1,42 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingPin\Desktop\trident classes\Roper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D8147E7-CAB3-4FED-8A62-318DA240D7E5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="8_{9D8147E7-CAB3-4FED-8A62-318DA240D7E5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="5" windowHeight="7680" windowWidth="21570" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="participantData" sheetId="1" r:id="rId1"/>
-    <sheet name="testScores" sheetId="4" r:id="rId2"/>
-    <sheet name="Referralsheet" sheetId="2" r:id="rId3"/>
-    <sheet name="Current Studies" sheetId="6" r:id="rId4"/>
-    <sheet name="OptInEamils" sheetId="3" r:id="rId5"/>
-    <sheet name="Formulas&amp;Tables" sheetId="5" r:id="rId6"/>
+    <sheet name="participantData" r:id="rId1" sheetId="1"/>
+    <sheet name="testScores" r:id="rId2" sheetId="4"/>
+    <sheet name="Referralsheet" r:id="rId3" sheetId="2"/>
+    <sheet name="Current Studies" r:id="rId4" sheetId="6"/>
+    <sheet name="OptInEamils" r:id="rId5" sheetId="3"/>
+    <sheet name="Formulas&amp;Tables" r:id="rId6" sheetId="5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable11" hidden="1">Referals[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable21" hidden="1">Table2</definedName>
+    <definedName hidden="1" name="_xlcn.WorksheetConnection_newdatabase.xlsxTable11">Referals[]</definedName>
+    <definedName hidden="1" name="_xlcn.WorksheetConnection_newdatabase.xlsxTable21">Table2</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+    <ext uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
       <x15:dataModel>
         <x15:modelTables>
-          <x15:modelTable id="Table2" name="Table2" connection="WorksheetConnection_new database.xlsx!Table2"/>
-          <x15:modelTable id="Table1" name="Table1" connection="WorksheetConnection_new database.xlsx!Table1"/>
+          <x15:modelTable connection="WorksheetConnection_new database.xlsx!Table2" id="Table2" name="Table2"/>
+          <x15:modelTable connection="WorksheetConnection_new database.xlsx!Table1" id="Table1" name="Table1"/>
         </x15:modelTables>
         <x15:modelRelationships>
-          <x15:modelRelationship fromTable="Table1" fromColumn="Column1" toTable="Table2" toColumn="Column1"/>
+          <x15:modelRelationship fromColumn="Column1" fromTable="Table1" toColumn="Column1" toTable="Table2"/>
         </x15:modelRelationships>
       </x15:dataModel>
     </ext>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t>Last Name</t>
   </si>
@@ -302,6 +302,33 @@
   </si>
   <si>
     <t>NIC</t>
+  </si>
+  <si>
+    <t>yost</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t>117 main street</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>29464</t>
+  </si>
+  <si>
+    <t>toastdroid@gmail.com</t>
+  </si>
+  <si>
+    <t>803-767-6643</t>
+  </si>
+  <si>
+    <t>Jimmy Johns</t>
+  </si>
+  <si>
+    <t>Bob evans</t>
   </si>
 </sst>
 </file>
@@ -352,51 +379,51 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt formatCode="0" numFmtId="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt formatCode="m/d/yyyy" numFmtId="19"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -409,94 +436,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Main" displayName="Main" ref="B3:X38" insertRowShift="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Main" id="3" insertRowShift="1" mc:Ignorable="xr xr3" name="Main" ref="B3:X38" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
   <autoFilter ref="B3:X38" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Last Name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="First Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOB" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="age" dataDxfId="6">
+    <tableColumn id="1" name="Last Name" xr3:uid="{00000000-0010-0000-0000-000001000000}"/>
+    <tableColumn id="2" name="First Name" xr3:uid="{00000000-0010-0000-0000-000002000000}"/>
+    <tableColumn dataDxfId="7" id="3" name="DOB" xr3:uid="{00000000-0010-0000-0000-000003000000}"/>
+    <tableColumn dataDxfId="6" id="4" name="age" xr3:uid="{00000000-0010-0000-0000-000004000000}">
       <calculatedColumnFormula>IF(ISBLANK(D4), "", (DATEDIF(D4, NOW(), "Y")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Race"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Gender"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Address"/>
-    <tableColumn id="20" xr3:uid="{A6CC2B3B-B730-4C77-8E1B-8524D8058490}" name="Address 2"/>
-    <tableColumn id="21" xr3:uid="{96274CA0-21F6-42F8-A6CC-1564219BEB3F}" name="City"/>
-    <tableColumn id="19" xr3:uid="{3564AF9A-9735-4F3E-B265-F58EE3E46F08}" name="State"/>
-    <tableColumn id="22" xr3:uid="{02668A8C-68D9-4CCB-B7C0-A7A59994786C}" name="Postal Code"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Email Address"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phone Number" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Test Date" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="W - Score" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="7s - Score" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Status" dataDxfId="1"/>
-    <tableColumn id="23" xr3:uid="{3F5E6B97-A5B9-4817-AC85-33BE5E2BCDF7}" name="Deseased" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="PCP"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Specialist"/>
-    <tableColumn id="25" xr3:uid="{98A49C78-82DD-424A-8F17-624EB4D4CC19}" name="Current Study"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Referral"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Mailing List"/>
+    <tableColumn id="5" name="Race" xr3:uid="{00000000-0010-0000-0000-000005000000}"/>
+    <tableColumn id="6" name="Gender" xr3:uid="{00000000-0010-0000-0000-000006000000}"/>
+    <tableColumn id="7" name="Address" xr3:uid="{00000000-0010-0000-0000-000007000000}"/>
+    <tableColumn id="20" name="Address 2" xr3:uid="{A6CC2B3B-B730-4C77-8E1B-8524D8058490}"/>
+    <tableColumn id="21" name="City" xr3:uid="{96274CA0-21F6-42F8-A6CC-1564219BEB3F}"/>
+    <tableColumn id="19" name="State" xr3:uid="{3564AF9A-9735-4F3E-B265-F58EE3E46F08}"/>
+    <tableColumn id="22" name="Postal Code" xr3:uid="{02668A8C-68D9-4CCB-B7C0-A7A59994786C}"/>
+    <tableColumn id="8" name="Email Address" xr3:uid="{00000000-0010-0000-0000-000008000000}"/>
+    <tableColumn dataDxfId="5" id="9" name="Phone Number" xr3:uid="{00000000-0010-0000-0000-000009000000}"/>
+    <tableColumn dataDxfId="4" id="15" name="Test Date" xr3:uid="{00000000-0010-0000-0000-00000F000000}"/>
+    <tableColumn dataDxfId="3" id="16" name="W - Score" xr3:uid="{00000000-0010-0000-0000-000010000000}"/>
+    <tableColumn dataDxfId="2" id="17" name="7s - Score" xr3:uid="{00000000-0010-0000-0000-000011000000}"/>
+    <tableColumn dataDxfId="1" id="14" name="Status" xr3:uid="{00000000-0010-0000-0000-00000E000000}"/>
+    <tableColumn dataDxfId="0" id="23" name="Deseased" xr3:uid="{3F5E6B97-A5B9-4817-AC85-33BE5E2BCDF7}"/>
+    <tableColumn id="10" name="PCP" xr3:uid="{00000000-0010-0000-0000-00000A000000}"/>
+    <tableColumn id="11" name="Specialist" xr3:uid="{00000000-0010-0000-0000-00000B000000}"/>
+    <tableColumn id="25" name="Current Study" xr3:uid="{98A49C78-82DD-424A-8F17-624EB4D4CC19}"/>
+    <tableColumn id="12" name="Referral" xr3:uid="{00000000-0010-0000-0000-00000C000000}"/>
+    <tableColumn id="13" name="Mailing List" xr3:uid="{00000000-0010-0000-0000-00000D000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TestScores" displayName="TestScores" ref="C3:K34" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="TestScores" id="4" mc:Ignorable="xr xr3" name="TestScores" ref="C3:K34" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}">
   <autoFilter ref="C3:K34" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Last Name"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="First Name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Test"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Date"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="W- score"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="7-score"/>
-    <tableColumn id="7" xr3:uid="{73A63323-73D0-4BD6-B700-273ED418AFD0}" name="CRD"/>
-    <tableColumn id="8" xr3:uid="{8C4C9C6C-D932-4492-83D9-EF8AA3B9594D}" name="LMD"/>
-    <tableColumn id="9" xr3:uid="{19D02257-082F-4200-B27E-1D6D79F59AD8}" name="Column3"/>
+    <tableColumn id="2" name="Last Name" xr3:uid="{00000000-0010-0000-0200-000002000000}"/>
+    <tableColumn id="1" name="First Name" xr3:uid="{00000000-0010-0000-0200-000001000000}"/>
+    <tableColumn id="4" name="Test" xr3:uid="{00000000-0010-0000-0200-000004000000}"/>
+    <tableColumn id="3" name="Date" xr3:uid="{00000000-0010-0000-0200-000003000000}"/>
+    <tableColumn id="5" name="W- score" xr3:uid="{00000000-0010-0000-0200-000005000000}"/>
+    <tableColumn id="6" name="7-score" xr3:uid="{00000000-0010-0000-0200-000006000000}"/>
+    <tableColumn id="7" name="CRD" xr3:uid="{73A63323-73D0-4BD6-B700-273ED418AFD0}"/>
+    <tableColumn id="8" name="LMD" xr3:uid="{8C4C9C6C-D932-4492-83D9-EF8AA3B9594D}"/>
+    <tableColumn id="9" name="Column3" xr3:uid="{19D02257-082F-4200-B27E-1D6D79F59AD8}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Referals" displayName="Referals" ref="B2:B30" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Referals" id="1" mc:Ignorable="xr xr3" name="Referals" ref="B2:B30" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}">
   <autoFilter ref="B2:B30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Referals"/>
+    <tableColumn id="1" name="Referals" xr3:uid="{00000000-0010-0000-0300-000001000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{58406E35-D93C-4D3E-88D6-AC79BD500D3A}" name="Studies" displayName="Studies" ref="B2:B11" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Studies" id="7" mc:Ignorable="xr xr3" name="Studies" ref="B2:B11" totalsRowShown="0" xr:uid="{58406E35-D93C-4D3E-88D6-AC79BD500D3A}">
   <autoFilter ref="B2:B11" xr:uid="{B1FCC2A1-DF48-4F79-8FCB-DB88BAFD76A8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FC3B7099-14D8-4512-9583-AF23E8DE88A0}" name="Studies"/>
+    <tableColumn id="1" name="Studies" xr3:uid="{FC3B7099-14D8-4512-9583-AF23E8DE88A0}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{937CA078-BB36-4EC9-8760-8D270CC5FAC5}" name="Emails" displayName="Emails" ref="B2:B32" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Emails" id="6" mc:Ignorable="xr xr3" name="Emails" ref="B2:B32" totalsRowShown="0" xr:uid="{937CA078-BB36-4EC9-8760-8D270CC5FAC5}">
   <autoFilter ref="B2:B32" xr:uid="{CD5E52FE-0FBA-4585-BB8A-AF0121AEA9E7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{37155562-77A4-43EE-A29A-0B1862B52782}" name="OptInEmails"/>
+    <tableColumn id="1" name="OptInEmails" xr3:uid="{37155562-77A4-43EE-A29A-0B1862B52782}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C5AD7D3A-236A-42F2-8BAD-957E12CE3E0B}" name="YesNo" displayName="YesNo" ref="G3:G6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="YesNo" id="5" mc:Ignorable="xr xr3" name="YesNo" ref="G3:G6" totalsRowShown="0" xr:uid="{C5AD7D3A-236A-42F2-8BAD-957E12CE3E0B}">
   <autoFilter ref="G3:G6" xr:uid="{F59ACE9F-D7BA-45D2-A818-2F906660C99A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9BE15266-1ADB-4610-9896-1E6F8723D194}" name="Column1"/>
+    <tableColumn id="1" name="Column1" xr3:uid="{9BE15266-1ADB-4610-9896-1E6F8723D194}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -505,10 +532,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -543,7 +570,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -578,7 +605,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -672,21 +699,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -703,7 +730,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -755,16 +782,16 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:AE38"/>
+  <dimension ref="B1:AF39"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="V4" sqref="V4"/>
@@ -772,26 +799,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="12" width="21.140625" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="2" customWidth="1"/>
-    <col min="15" max="17" width="16.5703125" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="31" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="24" customWidth="1"/>
-    <col min="21" max="22" width="18.7109375" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" customWidth="1"/>
-    <col min="28" max="28" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.28515625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="3" width="9.7109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="9.85546875" collapsed="false"/>
+    <col min="8" max="12" customWidth="true" width="21.140625" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="25.140625" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" style="2" width="16.5703125" collapsed="false"/>
+    <col min="15" max="17" customWidth="true" hidden="true" style="2" width="16.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" style="2" width="31.0" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" style="2" width="12.42578125" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="24.0" collapsed="false"/>
+    <col min="21" max="22" customWidth="true" width="18.7109375" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" width="20.42578125" collapsed="false"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="28.42578125" collapsed="false"/>
+    <col min="49" max="49" customWidth="true" width="11.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row customHeight="1" ht="15" r="1" spans="2:31" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="6" t="s">
         <v>52</v>
       </c>
@@ -1163,9 +1190,48 @@
       </c>
       <c r="O38"/>
     </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" t="n">
+        <v>33645.0</v>
+      </c>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39"/>
+      <c r="I39" t="s">
+        <v>77</v>
+      </c>
+      <c r="J39" t="s">
+        <v>78</v>
+      </c>
+      <c r="K39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L39" t="s">
+        <v>80</v>
+      </c>
+      <c r="M39" t="s">
+        <v>81</v>
+      </c>
+      <c r="P39" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>83</v>
+      </c>
+      <c r="S39"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1173,19 +1239,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D75DDE49-0DF0-4E20-9C93-4A048040F42D}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{D75DDE49-0DF0-4E20-9C93-4A048040F42D}">
           <x14:formula1>
             <xm:f>Referralsheet!$B$3:$B$30</xm:f>
           </x14:formula1>
           <xm:sqref>W4:W38</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F5948E2-1BF3-4171-99C5-7D3D68F37AD0}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{2F5948E2-1BF3-4171-99C5-7D3D68F37AD0}">
           <x14:formula1>
             <xm:f>'Current Studies'!$B$4:$B$11</xm:f>
           </x14:formula1>
           <xm:sqref>V4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3053FDD-2C11-42FF-B550-EA3C44BA6277}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{C3053FDD-2C11-42FF-B550-EA3C44BA6277}">
           <x14:formula1>
             <xm:f>'Formulas&amp;Tables'!$G$5:$G$6</xm:f>
           </x14:formula1>
@@ -1198,9 +1264,9 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="C2:K27"/>
+  <dimension ref="C2:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -1208,12 +1274,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="15.28515625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="13.42578125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="11.42578125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
@@ -1323,7 +1389,7 @@
       <c r="F27" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1331,9 +1397,9 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1341,7 +1407,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.42578125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -1494,7 +1560,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1502,8 +1568,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FA51D1-84BF-4F18-8CF3-D76920A1D960}">
-  <dimension ref="B2:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FA51D1-84BF-4F18-8CF3-D76920A1D960}">
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -1511,7 +1577,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="25.7109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1626,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1568,9 +1634,9 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B2"/>
+  <dimension ref="B2:C2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -1578,7 +1644,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -1587,7 +1653,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1595,9 +1661,9 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E28FDDA-5349-4591-8391-A89BA5844250}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E28FDDA-5349-4591-8391-A89BA5844250}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="C3:G6"/>
+  <dimension ref="C3:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
@@ -1631,7 +1697,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Reset combo box after clear
</commit_message>
<xml_diff>
--- a/java/RoperALZIntake/RoperSpreadSheet2.xlsx
+++ b/java/RoperALZIntake/RoperSpreadSheet2.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Last Name</t>
   </si>
@@ -314,6 +314,30 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>supper</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>29485</t>
+  </si>
+  <si>
+    <t>loop@email.com</t>
+  </si>
+  <si>
+    <t>8438221636</t>
+  </si>
+  <si>
+    <t>Dr Howard</t>
+  </si>
+  <si>
+    <t>Dr Fine</t>
   </si>
 </sst>
 </file>
@@ -367,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -377,6 +401,7 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -774,7 +799,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:Y5"/>
+  <dimension ref="B1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -782,23 +807,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.33203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="12.6640625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="10.5546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="3" width="9.6640625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="9.88671875" collapsed="false"/>
-    <col min="8" max="12" customWidth="true" width="21.109375" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="25.109375" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" style="2" width="16.5546875" collapsed="false"/>
-    <col min="15" max="17" customWidth="true" hidden="true" style="2" width="16.5546875" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" style="2" width="31.0" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" style="2" width="12.44140625" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="24.0" collapsed="false"/>
-    <col min="21" max="22" customWidth="true" width="18.6640625" collapsed="false"/>
-    <col min="23" max="23" customWidth="true" width="15.88671875" collapsed="false"/>
-    <col min="24" max="24" customWidth="true" width="20.44140625" collapsed="false"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="28.44140625" collapsed="false"/>
-    <col min="49" max="49" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="9.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="8" max="12" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="25.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="16.5546875" collapsed="true"/>
+    <col min="15" max="17" customWidth="true" hidden="true" style="2" width="16.5546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="2" width="31.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15" r="1" spans="2:24" x14ac:dyDescent="0.7">
@@ -936,7 +961,7 @@
       <c r="C5" t="s">
         <v>76</v>
       </c>
-      <c r="D5" t="n" s="7">
+      <c r="D5" s="7" t="n">
         <v>34305.0</v>
       </c>
       <c r="E5">
@@ -976,6 +1001,56 @@
         <v>77</v>
       </c>
       <c r="W5"/>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="n" s="8">
+        <v>25359.0</v>
+      </c>
+      <c r="E6">
+        <f>IF(ISBLANK(D6), "", (DATEDIF(D6, NOW(), "Y")))</f>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" t="s">
+        <v>84</v>
+      </c>
+      <c r="R6" t="s">
+        <v>78</v>
+      </c>
+      <c r="S6" t="s">
+        <v>78</v>
+      </c>
+      <c r="T6" t="s">
+        <v>85</v>
+      </c>
+      <c r="U6" t="s">
+        <v>86</v>
+      </c>
+      <c r="W6" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1022,12 +1097,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="15.88671875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.44140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="14.109375" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="11.44140625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.3">
@@ -1155,7 +1230,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.44140625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
@@ -1325,7 +1400,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="25.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="25.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
@@ -1392,7 +1467,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Sprerad sheet update for test
</commit_message>
<xml_diff>
--- a/java/RoperALZIntake/RoperSpreadSheet2.xlsx
+++ b/java/RoperALZIntake/RoperSpreadSheet2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\git\rsfh-alz-intake-b\java\RoperALZIntake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C8C87F-2D5E-431F-8226-5DC8EB08C7C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CFF334-206B-4660-A82F-8B64562346D7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Formulas&amp;Tables" sheetId="5" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable11" hidden="1">Referals[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable1" hidden="1">Referals[]</definedName>
     <definedName name="termReason">'Formulas&amp;Tables'!$B$3:$B$6</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -63,7 +63,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable11"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="127">
   <si>
     <t>Last Name</t>
   </si>
@@ -197,12 +197,6 @@
     <t>Word of Mouth</t>
   </si>
   <si>
-    <t>W- score</t>
-  </si>
-  <si>
-    <t>7-score</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Roper St. Francis Participant Data</t>
   </si>
   <si>
@@ -446,6 +437,9 @@
     <t>Study Paticipation Ended</t>
   </si>
   <si>
+    <t>Score</t>
+  </si>
+  <si>
     <t>termReason</t>
   </si>
   <si>
@@ -459,93 +453,14 @@
   </si>
   <si>
     <t>Study Completed</t>
-  </si>
-  <si>
-    <t>franks</t>
-  </si>
-  <si>
-    <t>kevin</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>1234 loop</t>
-  </si>
-  <si>
-    <t>summerville</t>
-  </si>
-  <si>
-    <t>sc</t>
-  </si>
-  <si>
-    <t>29485</t>
-  </si>
-  <si>
-    <t>loop@loop.com</t>
-  </si>
-  <si>
-    <t>843-843-8523</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>dr howard</t>
-  </si>
-  <si>
-    <t>dr fine</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Dementia (unspecified)</t>
-  </si>
-  <si>
-    <t>de fine</t>
-  </si>
-  <si>
-    <t>loop</t>
-  </si>
-  <si>
-    <t>loop loop</t>
-  </si>
-  <si>
-    <t>843-845-9632</t>
-  </si>
-  <si>
-    <t>843-843-9874</t>
-  </si>
-  <si>
-    <t>843-852-9651</t>
-  </si>
-  <si>
-    <t>843-822-1969</t>
-  </si>
-  <si>
-    <t>dR hOWARD</t>
-  </si>
-  <si>
-    <t>dR FINE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -572,7 +487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,17 +508,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -641,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -653,25 +611,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -808,7 +775,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table9" displayName="Table9" ref="B1:J2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table9" displayName="Table9" ref="B1:J2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="B1:J2" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="First Name"/>
@@ -826,23 +793,6 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TestScores" displayName="TestScores" ref="B1:I2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="B1:I2" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Last Name"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="First Name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Test"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Date"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="W- score"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="7-score"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="CDR"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="LMD"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Referals" displayName="Referals" ref="B2:B30" totalsRowShown="0">
   <autoFilter ref="B2:B30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
@@ -852,7 +802,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Studies" displayName="Studies" ref="B2:B11" totalsRowShown="0">
   <autoFilter ref="B2:B11" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="1">
@@ -862,7 +812,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Emails" displayName="Emails" ref="B2:B32" totalsRowShown="0">
   <autoFilter ref="B2:B32" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="1">
@@ -1136,17 +1086,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:AE9"/>
+  <dimension ref="B1:AE6"/>
   <sheetViews>
-    <sheetView topLeftCell="V3" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="R3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" customWidth="1"/>
     <col min="8" max="12" width="21.109375" customWidth="1"/>
@@ -1167,7 +1117,7 @@
   <sheetData>
     <row r="1" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B1" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -1240,16 +1190,16 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" t="s">
         <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>53</v>
       </c>
       <c r="M3" t="s">
         <v>4</v>
@@ -1258,19 +1208,19 @@
         <v>8</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="T3" t="s">
         <v>9</v>
@@ -1279,7 +1229,7 @@
         <v>10</v>
       </c>
       <c r="V3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="W3" t="s">
         <v>11</v>
@@ -1298,177 +1248,6 @@
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.3">
       <c r="AE6" s="5"/>
-    </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="15">
-        <v>25359</v>
-      </c>
-      <c r="E7">
-        <f ca="1">IF(ISBLANK(D7), "", (DATEDIF(D7, NOW(), "Y")))</f>
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H7" t="s">
-        <v>133</v>
-      </c>
-      <c r="J7" t="s">
-        <v>134</v>
-      </c>
-      <c r="K7" t="s">
-        <v>135</v>
-      </c>
-      <c r="L7" t="s">
-        <v>136</v>
-      </c>
-      <c r="M7" t="s">
-        <v>137</v>
-      </c>
-      <c r="N7" t="s">
-        <v>138</v>
-      </c>
-      <c r="R7" t="s">
-        <v>139</v>
-      </c>
-      <c r="S7" t="s">
-        <v>139</v>
-      </c>
-      <c r="T7" t="s">
-        <v>140</v>
-      </c>
-      <c r="U7" t="s">
-        <v>141</v>
-      </c>
-      <c r="W7" t="s">
-        <v>14</v>
-      </c>
-      <c r="X7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="16">
-        <v>25359</v>
-      </c>
-      <c r="E8">
-        <f ca="1">IF(ISBLANK(D8), "", (DATEDIF(D8, NOW(), "Y")))</f>
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J8" t="s">
-        <v>134</v>
-      </c>
-      <c r="K8" t="s">
-        <v>135</v>
-      </c>
-      <c r="L8" t="s">
-        <v>136</v>
-      </c>
-      <c r="M8" t="s">
-        <v>137</v>
-      </c>
-      <c r="N8" t="s">
-        <v>138</v>
-      </c>
-      <c r="R8" t="s">
-        <v>139</v>
-      </c>
-      <c r="S8" t="s">
-        <v>139</v>
-      </c>
-      <c r="T8" t="s">
-        <v>140</v>
-      </c>
-      <c r="U8" t="s">
-        <v>141</v>
-      </c>
-      <c r="W8" t="s">
-        <v>14</v>
-      </c>
-      <c r="X8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="17">
-        <v>25359</v>
-      </c>
-      <c r="E9">
-        <f ca="1">IF(ISBLANK(D9), "", (DATEDIF(D9, NOW(), "Y")))</f>
-        <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H9" t="s">
-        <v>133</v>
-      </c>
-      <c r="J9" t="s">
-        <v>134</v>
-      </c>
-      <c r="K9" t="s">
-        <v>135</v>
-      </c>
-      <c r="L9" t="s">
-        <v>136</v>
-      </c>
-      <c r="M9" t="s">
-        <v>137</v>
-      </c>
-      <c r="N9" t="s">
-        <v>152</v>
-      </c>
-      <c r="R9" t="s">
-        <v>139</v>
-      </c>
-      <c r="S9" t="s">
-        <v>139</v>
-      </c>
-      <c r="T9" t="s">
-        <v>153</v>
-      </c>
-      <c r="U9" t="s">
-        <v>154</v>
-      </c>
-      <c r="W9" t="s">
-        <v>14</v>
-      </c>
-      <c r="X9" t="s">
-        <v>142</v>
-      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1494,7 +1273,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>'Formulas&amp;Tables'!#REF!</xm:f>
+            <xm:f>'Formulas&amp;Tables'!$G$5:$G$6</xm:f>
           </x14:formula1>
           <xm:sqref>S4</xm:sqref>
         </x14:dataValidation>
@@ -1507,10 +1286,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,31 +1298,44 @@
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C4" s="1"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>128</v>
-      </c>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1553,18 +1345,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:AF4"/>
+  <dimension ref="B1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="20.109375" bestFit="1" customWidth="1"/>
@@ -1577,307 +1367,787 @@
     <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.5546875" customWidth="1"/>
     <col min="18" max="19" width="12" customWidth="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" customWidth="1"/>
     <col min="28" max="28" width="12" customWidth="1"/>
     <col min="31" max="31" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="N1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="O1" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="P1" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="S1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="U1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="V1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="X1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="T1" s="10" t="s">
+      <c r="Y1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF1" s="11" t="s">
-        <v>73</v>
+      <c r="AE1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="15">
-        <v>25359</v>
-      </c>
-      <c r="F2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J2" t="s">
-        <v>144</v>
-      </c>
-      <c r="K2" t="s">
-        <v>144</v>
-      </c>
-      <c r="L2" t="s">
-        <v>144</v>
-      </c>
-      <c r="M2" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" t="s">
-        <v>144</v>
-      </c>
-      <c r="O2" t="s">
-        <v>143</v>
-      </c>
-      <c r="P2" t="s">
-        <v>144</v>
-      </c>
-      <c r="S2" t="s">
-        <v>144</v>
-      </c>
-      <c r="V2" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>144</v>
-      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="17"/>
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="16">
-        <v>25359</v>
-      </c>
-      <c r="E3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="16">
-        <v>36550</v>
-      </c>
-      <c r="J3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K3" t="s">
-        <v>142</v>
-      </c>
-      <c r="L3" t="s">
-        <v>142</v>
-      </c>
-      <c r="M3" t="s">
-        <v>142</v>
-      </c>
-      <c r="N3" t="s">
-        <v>142</v>
-      </c>
-      <c r="O3" t="s">
-        <v>147</v>
-      </c>
-      <c r="P3" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="R3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="S3" t="s">
-        <v>142</v>
-      </c>
-      <c r="T3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="U3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="V3" t="s">
-        <v>142</v>
-      </c>
-      <c r="W3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="X3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>142</v>
-      </c>
-      <c r="Z3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="AA3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC3" s="16">
-        <v>43307.450627442129</v>
-      </c>
-      <c r="AD3" s="16">
-        <v>43307.450627442129</v>
-      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="20"/>
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="17">
-        <v>25359</v>
-      </c>
-      <c r="F4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="H4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J4" t="s">
-        <v>144</v>
-      </c>
-      <c r="K4" t="s">
-        <v>144</v>
-      </c>
-      <c r="L4" t="s">
-        <v>144</v>
-      </c>
-      <c r="M4" t="s">
-        <v>144</v>
-      </c>
-      <c r="N4" t="s">
-        <v>144</v>
-      </c>
-      <c r="O4" t="s">
-        <v>143</v>
-      </c>
-      <c r="P4" t="s">
-        <v>144</v>
-      </c>
-      <c r="S4" t="s">
-        <v>144</v>
-      </c>
-      <c r="V4" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>144</v>
-      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="17"/>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="20"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="17"/>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="20"/>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="17"/>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="19"/>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="19"/>
+      <c r="AE9" s="19"/>
+      <c r="AF9" s="20"/>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="16"/>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="16"/>
+      <c r="AE10" s="16"/>
+      <c r="AF10" s="17"/>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="20"/>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="16"/>
+      <c r="AC12" s="16"/>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="17"/>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="20"/>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="16"/>
+      <c r="AE14" s="16"/>
+      <c r="AF14" s="17"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="20"/>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="17"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
+      <c r="AE17" s="19"/>
+      <c r="AF17" s="20"/>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="16"/>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="16"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="16"/>
+      <c r="AF18" s="17"/>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="20"/>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="17"/>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>'Formulas&amp;Tables'!$G$4:$G$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I21 R2:R21 U2:U21 X2:X21 AA2:AA21 AD2:AD21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:L5"/>
+  <dimension ref="B1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
@@ -1889,157 +2159,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="I1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="12" t="s">
+      <c r="K1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="L1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J3" t="s">
-        <v>144</v>
-      </c>
-      <c r="K3" t="s">
-        <v>139</v>
-      </c>
-      <c r="L3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J4" t="s">
-        <v>144</v>
-      </c>
-      <c r="K4" t="s">
-        <v>148</v>
-      </c>
-      <c r="L4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" t="s">
-        <v>139</v>
-      </c>
-      <c r="I5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K5" t="s">
-        <v>139</v>
-      </c>
-      <c r="L5" t="s">
-        <v>143</v>
-      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2052,9 +2217,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
-            <xm:f>'Formulas&amp;Tables'!#REF!</xm:f>
+            <xm:f>'Formulas&amp;Tables'!$G$4:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2 G2 J2</xm:sqref>
+          <xm:sqref>D2 J2 G2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2064,9 +2229,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:J4"/>
+  <dimension ref="B1:J1"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -2091,112 +2256,25 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>89</v>
-      </c>
-      <c r="H1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" t="s">
-        <v>142</v>
-      </c>
-      <c r="J3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G4" t="s">
-        <v>143</v>
-      </c>
-      <c r="H4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J4" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2209,17 +2287,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:AA5"/>
+  <dimension ref="B1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+      <selection activeCell="B1" sqref="B1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
@@ -2239,163 +2317,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="25"/>
+      <c r="N1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" s="26"/>
+      <c r="T1" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18" t="s">
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="P1" s="19" t="s">
+      <c r="G2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="26"/>
+      <c r="O2" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="V2" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" s="19"/>
-      <c r="O2" s="13" t="s">
+      <c r="W2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA2" s="18"/>
+      <c r="Y2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA2" s="25"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="15">
-        <v>25359</v>
-      </c>
-    </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="16">
-        <v>25359</v>
-      </c>
+      <c r="E3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="17">
-        <v>25359</v>
-      </c>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="Q7" s="8"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="Q9" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2416,25 +2474,35 @@
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="Y1:Z1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="Z3:Z4" xr:uid="{00000000-0002-0000-0400-000000000000}">
-      <formula1>CHOICES</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Z5" xr:uid="{00000000-0002-0000-0400-000001000000}">
-      <formula1>termReason</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>'Formulas&amp;Tables'!$I$4:$I$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>AA3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+          <x14:formula1>
+            <xm:f>'Current Studies'!$B$4:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>R3:S3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:I2"/>
+  <dimension ref="B1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2442,45 +2510,77 @@
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E2" s="1"/>
+      <c r="D1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -2500,7 +2600,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -2670,47 +2770,47 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2737,7 +2837,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-mapped writer to remove two colums from spreadsheet
</commit_message>
<xml_diff>
--- a/java/RoperALZIntake/RoperSpreadSheet2.xlsx
+++ b/java/RoperALZIntake/RoperSpreadSheet2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\git\rsfh-alz-intake-b\java\RoperALZIntake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7413FFE9-728F-4041-BF16-D2280F7C7A13}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF84158-A1B1-4955-B5F4-D4B5FF2F9F5A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="153">
   <si>
     <t>Last Name</t>
   </si>
@@ -359,12 +359,6 @@
     <t>Clinician</t>
   </si>
   <si>
-    <t>Date of Diagnosis</t>
-  </si>
-  <si>
-    <t>Related Symptoms</t>
-  </si>
-  <si>
     <t>Difficulty Planning</t>
   </si>
   <si>
@@ -525,6 +519,18 @@
   </si>
   <si>
     <t>notes problems</t>
+  </si>
+  <si>
+    <t>kevin</t>
+  </si>
+  <si>
+    <t>summer</t>
+  </si>
+  <si>
+    <t>843-822-1636</t>
+  </si>
+  <si>
+    <t>Dementia (unspecified)</t>
   </si>
 </sst>
 </file>
@@ -629,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -654,6 +660,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1109,7 +1117,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:AW8"/>
+  <dimension ref="B1:AW10"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -1268,230 +1276,344 @@
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" s="14">
         <v>25359</v>
       </c>
       <c r="E5">
-        <f ca="1">IF(ISBLANK(D5), "", (DATEDIF(D5, NOW(), "Y")))</f>
+        <f t="shared" ref="E5:E10" ca="1" si="0">IF(ISBLANK(D5), "", (DATEDIF(D5, NOW(), "Y")))</f>
         <v>49</v>
       </c>
       <c r="F5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" t="s">
         <v>128</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>129</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>130</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>131</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>132</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>133</v>
       </c>
-      <c r="M5" t="s">
+      <c r="R5" t="s">
         <v>134</v>
       </c>
-      <c r="N5" t="s">
+      <c r="S5" t="s">
+        <v>134</v>
+      </c>
+      <c r="T5" t="s">
         <v>135</v>
       </c>
-      <c r="R5" t="s">
+      <c r="U5" t="s">
         <v>136</v>
-      </c>
-      <c r="S5" t="s">
-        <v>136</v>
-      </c>
-      <c r="T5" t="s">
-        <v>137</v>
-      </c>
-      <c r="U5" t="s">
-        <v>138</v>
       </c>
       <c r="W5" t="s">
         <v>13</v>
       </c>
       <c r="X5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D6" s="15">
         <v>25359</v>
       </c>
       <c r="E6">
-        <f ca="1">IF(ISBLANK(D6), "", (DATEDIF(D6, NOW(), "Y")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>49</v>
       </c>
       <c r="F6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" t="s">
         <v>128</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>129</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" t="s">
         <v>130</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>131</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>132</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>133</v>
       </c>
-      <c r="M6" t="s">
+      <c r="R6" t="s">
         <v>134</v>
       </c>
-      <c r="N6" t="s">
+      <c r="S6" t="s">
+        <v>134</v>
+      </c>
+      <c r="T6" t="s">
         <v>135</v>
       </c>
-      <c r="R6" t="s">
+      <c r="U6" t="s">
         <v>136</v>
-      </c>
-      <c r="S6" t="s">
-        <v>136</v>
-      </c>
-      <c r="T6" t="s">
-        <v>137</v>
-      </c>
-      <c r="U6" t="s">
-        <v>138</v>
       </c>
       <c r="W6" t="s">
         <v>13</v>
       </c>
       <c r="X6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D7" s="16">
         <v>25359</v>
       </c>
       <c r="E7">
-        <f ca="1">IF(ISBLANK(D7), "", (DATEDIF(D7, NOW(), "Y")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>49</v>
       </c>
       <c r="F7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" t="s">
         <v>128</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>129</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" t="s">
         <v>130</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>131</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>132</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>133</v>
       </c>
-      <c r="M7" t="s">
+      <c r="R7" t="s">
         <v>134</v>
       </c>
-      <c r="N7" t="s">
+      <c r="S7" t="s">
+        <v>134</v>
+      </c>
+      <c r="T7" t="s">
         <v>135</v>
       </c>
-      <c r="R7" t="s">
+      <c r="U7" t="s">
         <v>136</v>
-      </c>
-      <c r="S7" t="s">
-        <v>136</v>
-      </c>
-      <c r="T7" t="s">
-        <v>137</v>
-      </c>
-      <c r="U7" t="s">
-        <v>138</v>
       </c>
       <c r="W7" t="s">
         <v>13</v>
       </c>
       <c r="X7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D8" s="17">
         <v>25359</v>
       </c>
       <c r="E8">
-        <f ca="1">IF(ISBLANK(D8), "", (DATEDIF(D8, NOW(), "Y")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" t="s">
         <v>129</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
         <v>130</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>131</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>132</v>
       </c>
-      <c r="L8" t="s">
-        <v>133</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
+        <v>145</v>
+      </c>
+      <c r="R8" t="s">
         <v>134</v>
       </c>
-      <c r="N8" t="s">
-        <v>147</v>
-      </c>
-      <c r="R8" t="s">
-        <v>136</v>
-      </c>
       <c r="S8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="T8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="U8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="W8" t="s">
         <v>14</v>
       </c>
       <c r="X8" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="18">
+        <v>25329</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" t="s">
+        <v>150</v>
+      </c>
+      <c r="K9" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" t="s">
+        <v>131</v>
+      </c>
+      <c r="M9" t="s">
+        <v>132</v>
+      </c>
+      <c r="N9" t="s">
+        <v>151</v>
+      </c>
+      <c r="R9" t="s">
+        <v>134</v>
+      </c>
+      <c r="S9" t="s">
+        <v>134</v>
+      </c>
+      <c r="T9" t="s">
+        <v>138</v>
+      </c>
+      <c r="U9" t="s">
+        <v>138</v>
+      </c>
+      <c r="W9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="19">
+        <v>25329</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" t="s">
+        <v>128</v>
+      </c>
+      <c r="J10" t="s">
+        <v>150</v>
+      </c>
+      <c r="K10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" t="s">
+        <v>131</v>
+      </c>
+      <c r="M10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" t="s">
+        <v>151</v>
+      </c>
+      <c r="R10" t="s">
+        <v>134</v>
+      </c>
+      <c r="S10" t="s">
+        <v>134</v>
+      </c>
+      <c r="T10" t="s">
+        <v>138</v>
+      </c>
+      <c r="U10" t="s">
+        <v>138</v>
+      </c>
+      <c r="W10" t="s">
+        <v>13</v>
+      </c>
+      <c r="X10" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1545,31 +1667,31 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I6" s="6"/>
     </row>
@@ -1590,10 +1712,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:AF5"/>
+  <dimension ref="B1:AD7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1603,32 +1725,30 @@
     <col min="4" max="4" width="12.88671875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="12" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="12" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="36.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="12" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="12" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="36.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1645,415 +1765,521 @@
         <v>94</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="M1" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="O1" s="8" t="s">
-        <v>143</v>
+        <v>90</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="U1" s="8" t="s">
-        <v>69</v>
-      </c>
       <c r="V1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="X1" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="Y1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="AB1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AD1" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D2" s="14">
         <v>25359</v>
       </c>
       <c r="F2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" t="s">
-        <v>141</v>
-      </c>
-      <c r="L2" t="s">
-        <v>141</v>
-      </c>
-      <c r="M2" t="s">
-        <v>141</v>
-      </c>
       <c r="N2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O2" t="s">
-        <v>142</v>
-      </c>
-      <c r="P2" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q2" s="14">
+        <v>137</v>
+      </c>
+      <c r="O2" s="14">
         <v>43307.514220115743</v>
+      </c>
+      <c r="P2" s="14">
+        <v>43307.514220115743</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>137</v>
       </c>
       <c r="R2" s="14">
         <v>43307.514220115743</v>
       </c>
-      <c r="S2" t="s">
-        <v>139</v>
-      </c>
-      <c r="T2" s="14">
+      <c r="S2" s="14">
         <v>43307.514220115743</v>
+      </c>
+      <c r="T2" t="s">
+        <v>137</v>
       </c>
       <c r="U2" s="14">
         <v>43307.514220115743</v>
       </c>
-      <c r="V2" t="s">
-        <v>139</v>
-      </c>
-      <c r="W2" s="14">
+      <c r="V2" s="14">
         <v>43307.514220115743</v>
+      </c>
+      <c r="W2" t="s">
+        <v>137</v>
       </c>
       <c r="X2" s="14">
         <v>43307.514220115743</v>
       </c>
-      <c r="Y2" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z2" s="14">
-        <v>43307.514220115743</v>
+      <c r="Y2" s="14">
+        <v>43307.51422016204</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>137</v>
       </c>
       <c r="AA2" s="14">
         <v>43307.51422016204</v>
       </c>
-      <c r="AB2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC2" s="14">
+      <c r="AB2" s="14">
         <v>43307.51422016204</v>
       </c>
-      <c r="AD2" s="14">
-        <v>43307.51422016204</v>
-      </c>
-    </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D3" s="15">
         <v>25359</v>
       </c>
       <c r="F3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M3" t="s">
         <v>140</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" t="s">
-        <v>141</v>
-      </c>
-      <c r="L3" t="s">
-        <v>141</v>
-      </c>
-      <c r="M3" t="s">
-        <v>141</v>
-      </c>
       <c r="N3" t="s">
-        <v>139</v>
-      </c>
-      <c r="O3" t="s">
-        <v>142</v>
-      </c>
-      <c r="P3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q3" s="15">
+        <v>137</v>
+      </c>
+      <c r="O3" s="15">
         <v>43307.52427199074</v>
+      </c>
+      <c r="P3" s="15">
+        <v>43307.52427199074</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>137</v>
       </c>
       <c r="R3" s="15">
         <v>43307.52427199074</v>
       </c>
-      <c r="S3" t="s">
-        <v>139</v>
-      </c>
-      <c r="T3" s="15">
+      <c r="S3" s="15">
         <v>43307.52427199074</v>
+      </c>
+      <c r="T3" t="s">
+        <v>137</v>
       </c>
       <c r="U3" s="15">
         <v>43307.52427199074</v>
       </c>
-      <c r="V3" t="s">
-        <v>139</v>
-      </c>
-      <c r="W3" s="15">
+      <c r="V3" s="15">
         <v>43307.52427199074</v>
+      </c>
+      <c r="W3" t="s">
+        <v>137</v>
       </c>
       <c r="X3" s="15">
         <v>43307.52427199074</v>
       </c>
-      <c r="Y3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z3" s="15">
+      <c r="Y3" s="15">
         <v>43307.52427199074</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>137</v>
       </c>
       <c r="AA3" s="15">
         <v>43307.52427199074</v>
       </c>
-      <c r="AB3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC3" s="15">
+      <c r="AB3" s="15">
         <v>43307.52427199074</v>
       </c>
-      <c r="AD3" s="15">
-        <v>43307.52427199074</v>
-      </c>
-    </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D4" s="16">
         <v>25359</v>
       </c>
       <c r="F4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="16">
+        <v>36892</v>
+      </c>
+      <c r="H4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" t="s">
+        <v>139</v>
+      </c>
+      <c r="K4" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M4" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" t="s">
-        <v>139</v>
-      </c>
-      <c r="I4" s="16">
-        <v>36892</v>
-      </c>
-      <c r="J4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" t="s">
-        <v>141</v>
-      </c>
-      <c r="L4" t="s">
-        <v>141</v>
-      </c>
-      <c r="M4" t="s">
-        <v>141</v>
-      </c>
       <c r="N4" t="s">
-        <v>139</v>
-      </c>
-      <c r="O4" t="s">
-        <v>142</v>
-      </c>
-      <c r="P4" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q4" s="16">
+        <v>137</v>
+      </c>
+      <c r="O4" s="16">
         <v>43307.52450900463</v>
+      </c>
+      <c r="P4" s="16">
+        <v>43307.52450900463</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>137</v>
       </c>
       <c r="R4" s="16">
         <v>43307.52450900463</v>
       </c>
-      <c r="S4" t="s">
-        <v>139</v>
-      </c>
-      <c r="T4" s="16">
+      <c r="S4" s="16">
         <v>43307.52450900463</v>
+      </c>
+      <c r="T4" t="s">
+        <v>137</v>
       </c>
       <c r="U4" s="16">
         <v>43307.52450900463</v>
       </c>
-      <c r="V4" t="s">
-        <v>139</v>
-      </c>
-      <c r="W4" s="16">
+      <c r="V4" s="16">
         <v>43307.52450900463</v>
+      </c>
+      <c r="W4" t="s">
+        <v>137</v>
       </c>
       <c r="X4" s="16">
         <v>43307.52450900463</v>
       </c>
-      <c r="Y4" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z4" s="16">
+      <c r="Y4" s="16">
         <v>43307.52450900463</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>137</v>
       </c>
       <c r="AA4" s="16">
         <v>43307.52450900463</v>
       </c>
-      <c r="AB4" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC4" s="16">
+      <c r="AB4" s="16">
         <v>43307.52450900463</v>
       </c>
-      <c r="AD4" s="16">
-        <v>43307.52450900463</v>
-      </c>
-    </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="17">
         <v>25359</v>
       </c>
       <c r="E5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" s="17"/>
+        <v>142</v>
+      </c>
+      <c r="H5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="17">
+        <v>36557</v>
+      </c>
       <c r="J5" t="s">
-        <v>139</v>
-      </c>
-      <c r="K5" s="17">
-        <v>36557</v>
+        <v>137</v>
+      </c>
+      <c r="K5" t="s">
+        <v>137</v>
       </c>
       <c r="L5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O5" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="P5" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>149</v>
-      </c>
-      <c r="R5" t="s">
-        <v>139</v>
-      </c>
-      <c r="S5" s="17">
+        <v>137</v>
+      </c>
+      <c r="Q5" s="17">
         <v>43307.531770104164</v>
+      </c>
+      <c r="R5" s="17">
+        <v>43307.531770104164</v>
+      </c>
+      <c r="S5" t="s">
+        <v>137</v>
       </c>
       <c r="T5" s="17">
         <v>43307.531770104164</v>
       </c>
-      <c r="U5" t="s">
-        <v>139</v>
-      </c>
-      <c r="V5" s="17">
+      <c r="U5" s="17">
         <v>43307.531770104164</v>
+      </c>
+      <c r="V5" t="s">
+        <v>137</v>
       </c>
       <c r="W5" s="17">
         <v>43307.531770104164</v>
       </c>
-      <c r="X5" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y5" s="17">
+      <c r="X5" s="17">
         <v>43307.531770104164</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>137</v>
       </c>
       <c r="Z5" s="17">
         <v>43307.531770104164</v>
       </c>
-      <c r="AA5" t="s">
-        <v>139</v>
-      </c>
-      <c r="AB5" s="17">
+      <c r="AA5" s="17">
         <v>43307.531770104164</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>137</v>
       </c>
       <c r="AC5" s="17">
         <v>43307.531770104164</v>
       </c>
-      <c r="AD5" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE5" s="17">
+      <c r="AD5" s="17">
         <v>43307.531770104164</v>
       </c>
-      <c r="AF5" s="17">
-        <v>43307.531770104164</v>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="18">
+        <v>25329</v>
+      </c>
+      <c r="F6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" t="s">
+        <v>137</v>
+      </c>
+      <c r="I6" s="18">
+        <v>36892</v>
+      </c>
+      <c r="J6" t="s">
+        <v>137</v>
+      </c>
+      <c r="K6" t="s">
+        <v>137</v>
+      </c>
+      <c r="L6" t="s">
+        <v>139</v>
+      </c>
+      <c r="M6" t="s">
+        <v>139</v>
+      </c>
+      <c r="N6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O6" t="s">
+        <v>147</v>
+      </c>
+      <c r="P6" t="s">
+        <v>139</v>
+      </c>
+      <c r="S6" t="s">
+        <v>139</v>
+      </c>
+      <c r="V6" t="s">
+        <v>137</v>
+      </c>
+      <c r="W6" s="18">
+        <v>40544</v>
+      </c>
+      <c r="X6" s="18">
+        <v>40909</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="19">
+        <v>25329</v>
+      </c>
+      <c r="E7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" s="19">
+        <v>36892</v>
+      </c>
+      <c r="H7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I7" s="19">
+        <v>36892</v>
+      </c>
+      <c r="J7" t="s">
+        <v>137</v>
+      </c>
+      <c r="K7" t="s">
+        <v>137</v>
+      </c>
+      <c r="L7" t="s">
+        <v>139</v>
+      </c>
+      <c r="M7" t="s">
+        <v>139</v>
+      </c>
+      <c r="N7" t="s">
+        <v>137</v>
+      </c>
+      <c r="O7" t="s">
+        <v>147</v>
+      </c>
+      <c r="P7" t="s">
+        <v>139</v>
+      </c>
+      <c r="S7" t="s">
+        <v>139</v>
+      </c>
+      <c r="V7" t="s">
+        <v>137</v>
+      </c>
+      <c r="W7" s="19">
+        <v>40544</v>
+      </c>
+      <c r="X7" s="19">
+        <v>40909</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2063,7 +2289,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:L6"/>
+  <dimension ref="B1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
@@ -2124,142 +2350,212 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L6" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" t="s">
+        <v>139</v>
+      </c>
+      <c r="K8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L8" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2285,7 +2581,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:J5"/>
+  <dimension ref="B1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -2335,118 +2631,176 @@
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J5" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J7" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2459,7 +2813,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:AA6"/>
+  <dimension ref="B1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Z4" sqref="Z4"/>
@@ -2489,137 +2843,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="20"/>
+      <c r="N1" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="O1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" s="21"/>
+      <c r="T1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18" t="s">
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18" t="s">
+    </row>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P1" s="19" t="s">
+      <c r="H2" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="N2" s="19"/>
-      <c r="O2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
       <c r="R2" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S2" s="11" t="s">
         <v>45</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>45</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Y2" s="12" t="s">
         <v>45</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA2" s="18"/>
+        <v>114</v>
+      </c>
+      <c r="AA2" s="20"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="14">
         <v>25359</v>
@@ -2627,10 +2981,10 @@
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" s="15">
         <v>25359</v>
@@ -2638,10 +2992,10 @@
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="16">
         <v>25359</v>
@@ -2649,13 +3003,35 @@
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="17">
         <v>25359</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="18">
+        <v>25329</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="19">
+        <v>25329</v>
       </c>
     </row>
   </sheetData>
@@ -2678,7 +3054,7 @@
     <mergeCell ref="Y1:Z1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="Z3:Z6" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="Z3:Z8" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>termReason</formula1>
     </dataValidation>
   </dataValidations>
@@ -2705,59 +3081,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18" t="s">
+      <c r="E1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="18"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="13" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>45</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>45</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>45</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>